<commit_message>
progress on CE logic
I need to finish CE5 cases, then CE1 and CE2. I have file cases failing
in integration testing.
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20460" tabRatio="562"/>
@@ -2314,7 +2314,7 @@
     <t>bestest_space_cooling_equipment_performance_tests</t>
   </si>
   <si>
-    <t>BESTEST Cooling 06714a (updated unitary and oa)</t>
+    <t>BESTEST Cooling 06714b (variables for 300-500)</t>
   </si>
 </sst>
 </file>
@@ -6029,7 +6029,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
adding logic to have 0 oa for CE5xx cases
Also added CE400 unit test
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -2314,7 +2314,7 @@
     <t>bestest_space_cooling_equipment_performance_tests</t>
   </si>
   <si>
-    <t>BESTEST Cooling 06714b (variables for 300-500)</t>
+    <t>BESTEST Cooling 060728a (CE5 logic)</t>
   </si>
 </sst>
 </file>
@@ -6029,7 +6029,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
stub HE and CE reporting measures and scripts
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -2286,15 +2286,6 @@
     <t>../weather/USA_MA_Boston-Logan.Intl.AP.725090_TMY3.epw</t>
   </si>
   <si>
-    <t>BESTEST Building Thermal Envelope and Fabric Load Reports</t>
-  </si>
-  <si>
-    <t>BESTESTBuildingThermalEnvelopeAndFabricLoadReports</t>
-  </si>
-  <si>
-    <t>bestest_building_thermal_envelope_and_fabric_load_reports</t>
-  </si>
-  <si>
     <t xml:space="preserve">["CE100 - Base-Case Building and Mechanical System","CE110 - Reduced Outdoor Dry-Bulb Temperature","CE120 - Increased Thermostat Setpoint","CE130 - Low Part-Load Ratio","CE140 - Reduced Outdoor Dry-Bulb Temperature at Low Part-Load Ratio","CE150 - Latent Load at High Sensible Heat Ratio","CE160 - Increased Thermostat Setpoint at High Sensible Heat Ratio","CE165 - Variatino fo Thermostat Setpoint and Outdoor Dry-Bulb Temperature at High Sensible Heat Ratio","CE170 - Reduced Sensible Load","CE180 - Increased Latent Load","CE185 - Increased Outdoor Dry-Bulb Temperature at Low Sensible Heat Ratio","CE190 - Low Part-Load Ratio at Low Sensible Heat Ratio","CE195 - Increased Outdoor Dry-Bulb Temperature at Low Sensible Heat Rato and Low Part-Load Rato","CE200 - Full-Load Test at AHRI Conditions","CE300 - Base Case 15% OA","CE310 - High Latent Load","CE320 - Infiltration","CE330 - Outside Air","CE340 - Infil/OA Interaction","CE350 - Thermostat Set Up","CE360 - Undersize","CE400 - Temperature Control","CE410 - Compressor Lockout","CE420 - ODB Limit","CE430 - Enthalpy Control","CE440 - Outdoor Enthalpy Limit","CE500 - Base Case (0% OA)","CE510 - High PLR","CE520 - Low EDB 15C","CE522 - Low EDB 20C","CE530 - Dry Coil","CE540 - Dry Coil, Low EDB","CE545 - Dry Coil, High EDB"]
 </t>
   </si>
@@ -2314,16 +2305,32 @@
     <t>bestest_space_cooling_equipment_performance_tests</t>
   </si>
   <si>
-    <t>BESTEST Cooling 060729e (updated seed)</t>
+    <t>BESBESTEST CE Reporting</t>
+  </si>
+  <si>
+    <t>bestestce_reporting</t>
+  </si>
+  <si>
+    <t>BESTESTCEReporting</t>
+  </si>
+  <si>
+    <t>BESTEST Cooling 060804 (stub reporting measure)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2494,1576 +2501,1576 @@
   </borders>
   <cellStyleXfs count="1569">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4073,7 +4080,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4083,10 +4090,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -4095,7 +4102,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4120,43 +4127,47 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1569">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6658,7 +6669,7 @@
   <dimension ref="A1:Z53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6842,13 +6853,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="E4" s="36" t="s">
         <v>67</v>
@@ -6893,26 +6904,26 @@
       </c>
       <c r="H5" s="37"/>
       <c r="I5" s="37" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="K5" s="37" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="L5" s="37" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="M5" s="37" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="N5" s="37" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="O5" s="41"/>
       <c r="P5" s="43" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="Q5" s="41"/>
       <c r="R5" s="37" t="s">
@@ -6927,18 +6938,18 @@
       <c r="Y5" s="37"/>
       <c r="Z5" s="37"/>
     </row>
-    <row r="6" spans="1:26" s="39" customFormat="1" ht="15">
+    <row r="6" spans="1:26" s="46" customFormat="1" ht="15">
       <c r="A6" s="36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>748</v>
+        <v>754</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>749</v>
+        <v>756</v>
       </c>
       <c r="E6" s="36" t="s">
         <v>232</v>
@@ -6953,7 +6964,7 @@
       <c r="M6" s="40"/>
       <c r="N6" s="40"/>
       <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
+      <c r="P6" s="45"/>
       <c r="Q6" s="40"/>
       <c r="R6" s="36"/>
       <c r="S6" s="36"/>

</xml_diff>

<commit_message>
adding output variables for CE cases
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20460" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20460" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2218,9 +2218,6 @@
     <t>BESTESTCEReporting</t>
   </si>
   <si>
-    <t>BESTEST Cooling 060804 (stub reporting measure)</t>
-  </si>
-  <si>
     <t>bestest_ce_reporting</t>
   </si>
   <si>
@@ -2231,6 +2228,9 @@
   </si>
   <si>
     <t>bestest_ce_reporting.mean_zone_temperature</t>
+  </si>
+  <si>
+    <t>BESTEST Cooling 060805a (output variabes)</t>
   </si>
 </sst>
 </file>
@@ -5955,7 +5955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -6127,7 +6127,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>725</v>
+        <v>729</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>470</v>
@@ -6862,7 +6862,7 @@
         <v>723</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D6" s="36" t="s">
         <v>724</v>
@@ -8227,7 +8227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
@@ -8564,15 +8564,15 @@
     </row>
     <row r="11" spans="1:13" s="22" customFormat="1">
       <c r="A11" s="15" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
stub 5-3A spreadsheet data
Once registerValues are updated in the reporting measure it will
populate the Excel files.
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="746">
   <si>
     <t>type</t>
   </si>
@@ -2212,25 +2212,73 @@
     <t>bestest_space_cooling_equipment_performance_tests</t>
   </si>
   <si>
-    <t>BESBESTEST CE Reporting</t>
-  </si>
-  <si>
     <t>BESTESTCEReporting</t>
   </si>
   <si>
     <t>bestest_ce_reporting</t>
   </si>
   <si>
-    <t>Min Temp</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.mean_zone_temperature</t>
-  </si>
-  <si>
-    <t>BESTEST Cooling 060805a (output variabes)</t>
+    <t>bestest_ce_reporting.clg_energy_consumption_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.clg_energy_consumption_compressor</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.clg_energy_consumption_supply_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.clg_energy_consumption_condenser_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evaporator_coil_load_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evaporator_coil_load_sensible</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evaporator_coil_load_latent</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.zone_load_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.zone_load_sensible</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.zone_load_latent</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_mean_cop</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_mean_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_mean_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_max_cop</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_max_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_max_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_min_cop</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_min_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_min_humidity_ratio</t>
+  </si>
+  <si>
+    <t>BESTEST CE Reporting</t>
+  </si>
+  <si>
+    <t>BESTEST Cooling 060805c (stub CE5-3A reporting)</t>
   </si>
 </sst>
 </file>
@@ -2415,8 +2463,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1569">
+  <cellStyleXfs count="1571">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4085,7 +4135,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1569">
+  <cellStyles count="1571">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4870,6 +4920,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1564" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1566" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1570" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5654,6 +5705,7 @@
     <cellStyle name="Hyperlink" xfId="1563" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1565" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1569" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6127,7 +6179,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>729</v>
+        <v>745</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>470</v>
@@ -6585,7 +6637,7 @@
   <dimension ref="A1:Z53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6859,13 +6911,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="36" t="s">
+        <v>744</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>724</v>
+      </c>
+      <c r="D6" s="36" t="s">
         <v>723</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>725</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>724</v>
       </c>
       <c r="E6" s="36" t="s">
         <v>232</v>
@@ -8225,11 +8277,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M91"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8563,20 +8615,14 @@
       <c r="M10" s="15"/>
     </row>
     <row r="11" spans="1:13" s="22" customFormat="1">
-      <c r="A11" s="15" t="s">
-        <v>726</v>
-      </c>
+      <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>728</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>727</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>63</v>
-      </c>
+        <v>725</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="15" t="b">
         <v>1</v>
       </c>
@@ -8595,12 +8641,20 @@
       <c r="A12" s="15"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
+      <c r="D12" s="15" t="s">
+        <v>726</v>
+      </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
+      <c r="G12" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
@@ -8610,12 +8664,20 @@
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
+      <c r="D13" s="15" t="s">
+        <v>727</v>
+      </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
+      <c r="G13" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
@@ -8625,27 +8687,43 @@
       <c r="A14" s="15"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
+      <c r="D14" s="15" t="s">
+        <v>728</v>
+      </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
+      <c r="G14" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
     </row>
-    <row r="15" spans="1:13" s="22" customFormat="1">
+    <row r="15" spans="1:13" s="21" customFormat="1">
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
+      <c r="D15" s="15" t="s">
+        <v>729</v>
+      </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
+      <c r="G15" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
@@ -8655,12 +8733,20 @@
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
+      <c r="D16" s="15" t="s">
+        <v>730</v>
+      </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
+      <c r="G16" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
@@ -8670,12 +8756,20 @@
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
+      <c r="D17" s="15" t="s">
+        <v>731</v>
+      </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
+      <c r="G17" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
@@ -8685,12 +8779,20 @@
       <c r="A18" s="15"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
+      <c r="D18" s="15" t="s">
+        <v>732</v>
+      </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
+      <c r="G18" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
@@ -8700,12 +8802,20 @@
       <c r="A19" s="15"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
+      <c r="D19" s="15" t="s">
+        <v>733</v>
+      </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
+      <c r="G19" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
@@ -8715,27 +8825,43 @@
       <c r="A20" s="15"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
+      <c r="D20" s="15" t="s">
+        <v>734</v>
+      </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
+      <c r="G20" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
     </row>
-    <row r="21" spans="1:13" s="21" customFormat="1">
+    <row r="21" spans="1:13" s="22" customFormat="1">
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
+      <c r="D21" s="15" t="s">
+        <v>735</v>
+      </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
+      <c r="G21" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
@@ -8745,12 +8871,20 @@
       <c r="A22" s="15"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
+      <c r="D22" s="15" t="s">
+        <v>736</v>
+      </c>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
+      <c r="G22" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
@@ -8760,12 +8894,20 @@
       <c r="A23" s="15"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
+      <c r="D23" s="15" t="s">
+        <v>737</v>
+      </c>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
+      <c r="G23" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
@@ -8775,43 +8917,99 @@
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
+      <c r="D24" s="15" t="s">
+        <v>738</v>
+      </c>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
+      <c r="G24" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
       <c r="M24" s="15"/>
     </row>
-    <row r="25" spans="1:13" s="22" customFormat="1">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
+    <row r="25" spans="1:13">
+      <c r="B25" s="21"/>
+      <c r="D25" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="G25" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:13">
       <c r="B26" s="21"/>
+      <c r="D26" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="G26" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:13">
       <c r="B27" s="21"/>
+      <c r="D27" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="G27" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:13">
       <c r="B28" s="21"/>
+      <c r="D28" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="G28" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:13">
       <c r="B29" s="21"/>
+      <c r="D29" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="G29" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:13">
       <c r="B30" s="21"/>
@@ -8995,9 +9193,6 @@
     </row>
     <row r="90" spans="2:2">
       <c r="B90" s="21"/>
-    </row>
-    <row r="91" spans="2:2">
-      <c r="B91" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update CE reporting measure and spreadsheet
Still need to run/test on server and update results csv
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2251" uniqueCount="839">
   <si>
     <t>type</t>
   </si>
@@ -2278,14 +2278,293 @@
     <t>BESTEST CE Reporting</t>
   </si>
   <si>
-    <t>BESTEST Cooling 060805c (stub CE5-3A reporting)</t>
+    <t>bestest_ce_reporting.ann_sum_evap_coil_load_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_sum_evap_coil_load_sensible</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_sum_evap_coil_load_latent</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_mean_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_mean_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_mean_zone_relative_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_mean_odb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_mean_outdoor_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_sum_clg_consumption_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_sum_clg_consumption_compressor</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_sum_clg_consumption_cond_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_sum_clg_consumption_indoor_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_sum_evap_coil_load_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_sum_evap_coil_load_sensible</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_sum_evap_coil_load_latent</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_mean_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_mean_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_mean_zone_relative_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.energy_consumption_comp_both_fans_wh</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.energy_consumption_comp_both_fans_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.energy_consumption_comp_both_fans_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_sensible_wh</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_sensible_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_sensible_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_latent_wh</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_latent_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_latent_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_sensible_and_latent_wh</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_sensible_and_latent_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_sensible_and_latent_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.weather_odb_c</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.weather_odb_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.weather_odb_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.weather_outdoor_humidity_ratio_c</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.weather_outdoor_humidity_ratio_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.weather_outdoor_humidity_ratio_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.cop2_max_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.cop2_max_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.cop2_max_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.cop2_min_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.cop2_min_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.cop2_min_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.idb_max_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.idb_max_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.idb_max_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.idb_min_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.idb_min_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.idb_min_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.hr_max_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.hr_max_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.hr_max_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.hr_min_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.hr_min_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.hr_min_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.rh_max_relative_humidity</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.rh_max_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.rh_max_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.rh_min_relative_humidity</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.rh_min_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.rh_min_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_energy_consumpton_compressor</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_energy_consumpton_cond_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_evaporator_coil_load_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_evaporator_coil_load_sensible</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_evaporator_coil_load_latent</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_zone_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_odb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_edb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_ewb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_outdoor_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_energy_consumption_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_energy_consumption_compressor</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_energy_consumption_supply_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_energy_consumption_condenser_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_evaporator_coil_load_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_evaporator_coil_load_sensible</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_evaporator_coil_load_latent</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_zone_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_odb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_edb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_energy_consumption_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_energy_consumption_compressor</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_energy_consumption_supply_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_energy_consumption_condenser_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_evaporator_coil_load_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_evaporator_coil_load_sensible</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_evaporator_coil_load_latent</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_zone_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_odb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_edb</t>
+  </si>
+  <si>
+    <t>BESTEST Cooling 060812a (stub CE5-3B reporting)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2357,6 +2636,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
     </font>
   </fonts>
   <fills count="15">
@@ -2463,7 +2747,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1571">
+  <cellStyleXfs count="1589">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4035,8 +4319,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4134,8 +4436,11 @@
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1571">
+  <cellStyles count="1589">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4921,6 +5226,15 @@
     <cellStyle name="Followed Hyperlink" xfId="1566" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1568" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1588" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5706,6 +6020,15 @@
     <cellStyle name="Hyperlink" xfId="1565" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1567" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1577" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1579" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1587" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6179,7 +6502,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>745</v>
+        <v>838</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>470</v>
@@ -6637,7 +6960,7 @@
   <dimension ref="A1:Z53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8277,11 +8600,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M90"/>
+  <dimension ref="A1:M122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9010,189 +9333,1370 @@
       <c r="I29" s="15" t="b">
         <v>0</v>
       </c>
+      <c r="J29" s="47"/>
     </row>
     <row r="30" spans="1:13">
       <c r="B30" s="21"/>
+      <c r="D30" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="G30" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:13">
       <c r="B31" s="21"/>
+      <c r="D31" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="G31" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:13">
       <c r="B32" s="21"/>
-    </row>
-    <row r="33" spans="2:2">
+      <c r="D32" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="G32" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9">
       <c r="B33" s="21"/>
-    </row>
-    <row r="34" spans="2:2">
+      <c r="D33" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="G33" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
       <c r="B34" s="21"/>
-    </row>
-    <row r="35" spans="2:2">
+      <c r="D34" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="G34" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9">
       <c r="B35" s="21"/>
-    </row>
-    <row r="36" spans="2:2">
+      <c r="D35" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="G35" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9">
       <c r="B36" s="21"/>
-    </row>
-    <row r="37" spans="2:2">
+      <c r="D36" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="G36" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
       <c r="B37" s="21"/>
-    </row>
-    <row r="38" spans="2:2">
+      <c r="D37" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="G37" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9">
       <c r="B38" s="21"/>
-    </row>
-    <row r="39" spans="2:2">
+      <c r="D38" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="G38" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9">
       <c r="B39" s="21"/>
-    </row>
-    <row r="40" spans="2:2">
+      <c r="D39" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="G39" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
       <c r="B40" s="21"/>
-    </row>
-    <row r="41" spans="2:2">
+      <c r="D40" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="G40" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9">
       <c r="B41" s="21"/>
-    </row>
-    <row r="42" spans="2:2">
+      <c r="D41" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="G41" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9">
       <c r="B42" s="21"/>
-    </row>
-    <row r="43" spans="2:2">
+      <c r="D42" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G42" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9">
       <c r="B43" s="21"/>
-    </row>
-    <row r="44" spans="2:2">
+      <c r="D43" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="G43" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9">
       <c r="B44" s="21"/>
-    </row>
-    <row r="45" spans="2:2">
+      <c r="D44" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="G44" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9">
       <c r="B45" s="21"/>
-    </row>
-    <row r="46" spans="2:2">
+      <c r="D45" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="G45" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9">
       <c r="B46" s="21"/>
-    </row>
-    <row r="47" spans="2:2">
+      <c r="D46" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="G46" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I46" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9">
       <c r="B47" s="21"/>
-    </row>
-    <row r="48" spans="2:2">
+      <c r="D47" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="G47" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9">
       <c r="B48" s="21"/>
-    </row>
-    <row r="49" spans="2:2">
+      <c r="D48" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="G48" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9">
       <c r="B49" s="21"/>
-    </row>
-    <row r="50" spans="2:2">
+      <c r="D49" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="G49" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I49" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9">
       <c r="B50" s="21"/>
-    </row>
-    <row r="51" spans="2:2">
+      <c r="D50" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="G50" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9">
       <c r="B51" s="21"/>
-    </row>
-    <row r="52" spans="2:2">
+      <c r="D51" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="G51" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I51" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9">
       <c r="B52" s="21"/>
-    </row>
-    <row r="53" spans="2:2">
+      <c r="D52" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="G52" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H52" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I52" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9">
       <c r="B53" s="21"/>
-    </row>
-    <row r="54" spans="2:2">
+      <c r="D53" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="G53" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I53" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9">
       <c r="B54" s="21"/>
-    </row>
-    <row r="55" spans="2:2">
+      <c r="D54" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="G54" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I54" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9">
       <c r="B55" s="21"/>
-    </row>
-    <row r="56" spans="2:2">
+      <c r="D55" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="G55" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I55" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9">
       <c r="B56" s="21"/>
-    </row>
-    <row r="57" spans="2:2">
+      <c r="D56" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="G56" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I56" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9">
       <c r="B57" s="21"/>
-    </row>
-    <row r="58" spans="2:2">
+      <c r="D57" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="G57" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H57" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I57" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9">
       <c r="B58" s="21"/>
-    </row>
-    <row r="59" spans="2:2">
+      <c r="D58" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="G58" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H58" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I58" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9">
       <c r="B59" s="21"/>
-    </row>
-    <row r="60" spans="2:2">
+      <c r="D59" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="G59" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H59" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I59" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9">
       <c r="B60" s="21"/>
-    </row>
-    <row r="61" spans="2:2">
+      <c r="D60" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="G60" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H60" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I60" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9">
       <c r="B61" s="21"/>
-    </row>
-    <row r="62" spans="2:2">
+      <c r="D61" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="G61" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H61" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I61" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9">
       <c r="B62" s="21"/>
-    </row>
-    <row r="63" spans="2:2">
+      <c r="D62" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="G62" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H62" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I62" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9">
       <c r="B63" s="21"/>
-    </row>
-    <row r="64" spans="2:2">
+      <c r="D63" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="G63" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H63" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I63" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9">
       <c r="B64" s="21"/>
-    </row>
-    <row r="65" spans="2:2">
+      <c r="D64" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="G64" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H64" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I64" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9">
       <c r="B65" s="21"/>
-    </row>
-    <row r="66" spans="2:2">
+      <c r="D65" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="G65" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H65" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I65" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9">
       <c r="B66" s="21"/>
-    </row>
-    <row r="67" spans="2:2">
+      <c r="D66" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="G66" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H66" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I66" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9">
       <c r="B67" s="21"/>
-    </row>
-    <row r="68" spans="2:2">
+      <c r="D67" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="G67" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H67" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I67" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9">
       <c r="B68" s="21"/>
-    </row>
-    <row r="69" spans="2:2">
+      <c r="D68" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="G68" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H68" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I68" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9">
       <c r="B69" s="21"/>
-    </row>
-    <row r="70" spans="2:2">
+      <c r="D69" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="G69" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H69" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I69" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9">
       <c r="B70" s="21"/>
-    </row>
-    <row r="71" spans="2:2">
+      <c r="D70" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="G70" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H70" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I70" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9">
       <c r="B71" s="21"/>
-    </row>
-    <row r="72" spans="2:2">
+      <c r="D71" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="G71" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H71" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I71" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9">
       <c r="B72" s="21"/>
-    </row>
-    <row r="73" spans="2:2">
+      <c r="D72" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="G72" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H72" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I72" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9">
       <c r="B73" s="21"/>
-    </row>
-    <row r="74" spans="2:2">
+      <c r="D73" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="G73" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H73" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I73" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9">
       <c r="B74" s="21"/>
-    </row>
-    <row r="75" spans="2:2">
+      <c r="D74" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="G74" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H74" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I74" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9">
       <c r="B75" s="21"/>
-    </row>
-    <row r="76" spans="2:2">
+      <c r="D75" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="G75" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H75" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I75" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9">
       <c r="B76" s="21"/>
-    </row>
-    <row r="77" spans="2:2">
+      <c r="D76" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="G76" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H76" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I76" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9">
       <c r="B77" s="21"/>
-    </row>
-    <row r="78" spans="2:2">
+      <c r="D77" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="G77" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H77" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I77" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9">
       <c r="B78" s="21"/>
-    </row>
-    <row r="79" spans="2:2">
+      <c r="D78" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="G78" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H78" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I78" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9">
       <c r="B79" s="21"/>
-    </row>
-    <row r="80" spans="2:2">
+      <c r="D79" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="G79" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H79" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I79" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9">
       <c r="B80" s="21"/>
-    </row>
-    <row r="81" spans="2:2">
+      <c r="D80" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="G80" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H80" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I80" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9">
       <c r="B81" s="21"/>
-    </row>
-    <row r="82" spans="2:2">
+      <c r="D81" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="G81" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H81" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I81" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9">
       <c r="B82" s="21"/>
-    </row>
-    <row r="83" spans="2:2">
+      <c r="D82" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="G82" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H82" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I82" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9">
       <c r="B83" s="21"/>
-    </row>
-    <row r="84" spans="2:2">
+      <c r="D83" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="G83" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H83" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I83" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9">
       <c r="B84" s="21"/>
-    </row>
-    <row r="85" spans="2:2">
+      <c r="D84" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="G84" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H84" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I84" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9">
       <c r="B85" s="21"/>
-    </row>
-    <row r="86" spans="2:2">
+      <c r="D85" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="G85" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H85" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I85" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9">
       <c r="B86" s="21"/>
-    </row>
-    <row r="87" spans="2:2">
+      <c r="D86" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="G86" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H86" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I86" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9">
       <c r="B87" s="21"/>
-    </row>
-    <row r="88" spans="2:2">
+      <c r="D87" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="G87" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H87" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I87" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9">
       <c r="B88" s="21"/>
-    </row>
-    <row r="89" spans="2:2">
+      <c r="D88" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="G88" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H88" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I88" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9">
       <c r="B89" s="21"/>
-    </row>
-    <row r="90" spans="2:2">
+      <c r="D89" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="G89" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H89" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I89" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9">
       <c r="B90" s="21"/>
+      <c r="D90" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="G90" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H90" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I90" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9">
+      <c r="D91" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="G91" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H91" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I91" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9">
+      <c r="D92" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="G92" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H92" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I92" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="2:9">
+      <c r="D93" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="G93" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H93" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I93" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:9">
+      <c r="D94" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="G94" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H94" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I94" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:9">
+      <c r="D95" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="G95" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H95" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I95" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9">
+      <c r="D96" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="G96" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H96" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I96" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="4:9">
+      <c r="D97" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="G97" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H97" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I97" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="4:9">
+      <c r="D98" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="G98" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H98" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I98" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="4:9">
+      <c r="D99" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="G99" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H99" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I99" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="4:9">
+      <c r="D100" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="G100" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H100" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I100" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="4:9">
+      <c r="D101" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G101" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H101" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I101" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="4:9">
+      <c r="D102" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="G102" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H102" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I102" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="4:9">
+      <c r="D103" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="G103" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H103" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I103" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="4:9">
+      <c r="D104" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="G104" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H104" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I104" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="4:9">
+      <c r="D105" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="G105" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H105" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I105" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="4:9">
+      <c r="D106" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="G106" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H106" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I106" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="4:9">
+      <c r="D107" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="G107" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H107" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I107" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="4:9">
+      <c r="D108" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="G108" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H108" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I108" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="4:9">
+      <c r="D109" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="G109" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H109" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I109" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="4:9">
+      <c r="D110" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="G110" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H110" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I110" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="4:9">
+      <c r="D111" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="G111" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H111" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I111" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="4:9">
+      <c r="D112" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="G112" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H112" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I112" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="4:9">
+      <c r="D113" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="G113" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H113" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I113" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="4:9">
+      <c r="D114" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="G114" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H114" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I114" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="4:9">
+      <c r="D115" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="G115" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H115" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I115" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="4:9">
+      <c r="D116" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="G116" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H116" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I116" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="4:9">
+      <c r="D117" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="G117" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H117" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I117" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="4:9">
+      <c r="D118" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="G118" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H118" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I118" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="4:9">
+      <c r="D119" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="G119" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H119" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I119" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="4:9">
+      <c r="D120" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="G120" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H120" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I120" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="4:9">
+      <c r="D121" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="G121" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H121" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I121" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="4:9">
+      <c r="D122" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="G122" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H122" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I122" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
csv looks good off of server
Now I need to clean up errors on  ce results script. It is failing
looking for CE525 that is in spreadsheet but not in cases in measure.
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -2557,7 +2557,7 @@
     <t>bestest_ce_reporting.0625_day_edb</t>
   </si>
   <si>
-    <t>BESTEST Cooling 060812a (stub CE5-3B reporting)</t>
+    <t>BESTEST Cooling 060812c (fix registerValue name)</t>
   </si>
 </sst>
 </file>
@@ -4433,11 +4433,11 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1589">
@@ -7016,14 +7016,14 @@
       <c r="R1" s="29"/>
       <c r="S1" s="26"/>
       <c r="T1" s="26"/>
-      <c r="U1" s="46" t="s">
+      <c r="U1" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15">
       <c r="A2" s="30" t="s">
@@ -8603,8 +8603,8 @@
   <dimension ref="A1:M122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9333,7 +9333,7 @@
       <c r="I29" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="J29" s="47"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:13">
       <c r="B30" s="21"/>

</xml_diff>

<commit_message>
All 5-3B values stubbed except for two tables
I commented out two tables I need to fix bug in.
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2251" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="845">
   <si>
     <t>type</t>
   </si>
@@ -2193,371 +2193,389 @@
     <t>../weather/USA_MA_Boston-Logan.Intl.AP.725090_TMY3.epw</t>
   </si>
   <si>
-    <t xml:space="preserve">["CE100 - Base-Case Building and Mechanical System","CE110 - Reduced Outdoor Dry-Bulb Temperature","CE120 - Increased Thermostat Setpoint","CE130 - Low Part-Load Ratio","CE140 - Reduced Outdoor Dry-Bulb Temperature at Low Part-Load Ratio","CE150 - Latent Load at High Sensible Heat Ratio","CE160 - Increased Thermostat Setpoint at High Sensible Heat Ratio","CE165 - Variatino fo Thermostat Setpoint and Outdoor Dry-Bulb Temperature at High Sensible Heat Ratio","CE170 - Reduced Sensible Load","CE180 - Increased Latent Load","CE185 - Increased Outdoor Dry-Bulb Temperature at Low Sensible Heat Ratio","CE190 - Low Part-Load Ratio at Low Sensible Heat Ratio","CE195 - Increased Outdoor Dry-Bulb Temperature at Low Sensible Heat Rato and Low Part-Load Rato","CE200 - Full-Load Test at AHRI Conditions","CE300 - Base Case 15% OA","CE310 - High Latent Load","CE320 - Infiltration","CE330 - Outside Air","CE340 - Infil/OA Interaction","CE350 - Thermostat Set Up","CE360 - Undersize","CE400 - Temperature Control","CE410 - Compressor Lockout","CE420 - ODB Limit","CE430 - Enthalpy Control","CE440 - Outdoor Enthalpy Limit","CE500 - Base Case (0% OA)","CE510 - High PLR","CE520 - Low EDB 15C","CE522 - Low EDB 20C","CE530 - Dry Coil","CE540 - Dry Coil, Low EDB","CE545 - Dry Coil, High EDB"]
+    <t>CE100 - Base-Case Building and Mechanical System</t>
+  </si>
+  <si>
+    <t>|CE100 - Base-Case Building and Mechanical System|</t>
+  </si>
+  <si>
+    <t>BESTEST Space Cooling Equipment Performance Tests</t>
+  </si>
+  <si>
+    <t>BESTESTSpaceCoolingEquipmentPerformanceTests</t>
+  </si>
+  <si>
+    <t>bestest_space_cooling_equipment_performance_tests</t>
+  </si>
+  <si>
+    <t>BESTESTCEReporting</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.clg_energy_consumption_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.clg_energy_consumption_compressor</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.clg_energy_consumption_supply_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.clg_energy_consumption_condenser_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evaporator_coil_load_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evaporator_coil_load_sensible</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evaporator_coil_load_latent</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.zone_load_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.zone_load_sensible</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.zone_load_latent</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_mean_cop</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_mean_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_mean_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_max_cop</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_max_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_max_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_min_cop</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_min_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.feb_min_humidity_ratio</t>
+  </si>
+  <si>
+    <t>BESTEST CE Reporting</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_sum_evap_coil_load_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_sum_evap_coil_load_sensible</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_sum_evap_coil_load_latent</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_mean_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_mean_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_mean_odb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_mean_outdoor_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_sum_clg_consumption_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_sum_clg_consumption_compressor</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_sum_clg_consumption_cond_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_sum_clg_consumption_indoor_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_sum_evap_coil_load_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_sum_evap_coil_load_sensible</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_sum_evap_coil_load_latent</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_mean_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_mean_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.energy_consumption_comp_both_fans_wh</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.energy_consumption_comp_both_fans_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.energy_consumption_comp_both_fans_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_sensible_wh</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_sensible_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_sensible_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_latent_wh</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_latent_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_latent_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_sensible_and_latent_wh</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_sensible_and_latent_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.evap_coil_load_sensible_and_latent_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.weather_odb_c</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.weather_odb_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.weather_odb_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.weather_outdoor_humidity_ratio_c</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.weather_outdoor_humidity_ratio_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.weather_outdoor_humidity_ratio_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.cop2_max_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.cop2_max_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.cop2_max_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.cop2_min_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.cop2_min_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.cop2_min_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.idb_max_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.idb_max_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.idb_max_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.idb_min_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.idb_min_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.idb_min_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.hr_max_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.hr_max_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.hr_max_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.hr_min_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.hr_min_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.hr_min_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.rh_max_relative_humidity</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.rh_max_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.rh_max_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.rh_min_relative_humidity</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.rh_min_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.rh_min_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_energy_consumpton_compressor</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_energy_consumpton_cond_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_evaporator_coil_load_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_evaporator_coil_load_sensible</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_evaporator_coil_load_latent</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_zone_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_odb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_edb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_ewb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0628_hourly_outdoor_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_energy_consumption_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_energy_consumption_compressor</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_energy_consumption_supply_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_energy_consumption_condenser_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_evaporator_coil_load_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_evaporator_coil_load_sensible</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_evaporator_coil_load_latent</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_zone_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_odb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0430_day_edb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_energy_consumption_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_energy_consumption_compressor</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_energy_consumption_supply_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_energy_consumption_condenser_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_evaporator_coil_load_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_evaporator_coil_load_sensible</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_evaporator_coil_load_latent</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_zone_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_odb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.0625_day_edb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">["CE100 - Base-Case Building and Mechanical System","CE110 - Reduced Outdoor Dry-Bulb Temperature","CE120 - Increased Thermostat Setpoint","CE130 - Low Part-Load Ratio","CE140 - Reduced Outdoor Dry-Bulb Temperature at Low Part-Load Ratio","CE150 - Latent Load at High Sensible Heat Ratio","CE160 - Increased Thermostat Setpoint at High Sensible Heat Ratio","CE165 - Variatino fo Thermostat Setpoint and Outdoor Dry-Bulb Temperature at High Sensible Heat Ratio","CE170 - Reduced Sensible Load","CE180 - Increased Latent Load","CE185 - Increased Outdoor Dry-Bulb Temperature at Low Sensible Heat Ratio","CE190 - Low Part-Load Ratio at Low Sensible Heat Ratio","CE195 - Increased Outdoor Dry-Bulb Temperature at Low Sensible Heat Rato and Low Part-Load Rato","CE200 - Full-Load Test at AHRI Conditions","CE300 - Base Case 15% OA","CE310 - High Latent Load","CE320 - Infiltration","CE330 - Outside Air","CE340 - Infil/OA Interaction","CE350 - Thermostat Set Up","CE360 - Undersize","CE400 - Temperature Control","CE410 - Compressor Lockout","CE420 - ODB Limit","CE430 - Enthalpy Control","CE440 - Outdoor Enthalpy Limit","CE500 - Base Case (0% OA)","CE510 - High PLR","CE520 - Low EDB 15C","CE522 - Low EDB 20C","CE525 - High EDB","CE530 - Dry Coil","CE540 - Dry Coil, Low EDB","CE545 - Dry Coil, High EDB"]
 </t>
   </si>
   <si>
-    <t>CE100 - Base-Case Building and Mechanical System</t>
-  </si>
-  <si>
-    <t>|CE100 - Base-Case Building and Mechanical System|</t>
-  </si>
-  <si>
-    <t>BESTEST Space Cooling Equipment Performance Tests</t>
-  </si>
-  <si>
-    <t>BESTESTSpaceCoolingEquipmentPerformanceTests</t>
-  </si>
-  <si>
-    <t>bestest_space_cooling_equipment_performance_tests</t>
-  </si>
-  <si>
-    <t>BESTESTCEReporting</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.clg_energy_consumption_total</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.clg_energy_consumption_compressor</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.clg_energy_consumption_supply_fan</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.clg_energy_consumption_condenser_fan</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.evaporator_coil_load_total</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.evaporator_coil_load_sensible</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.evaporator_coil_load_latent</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.zone_load_total</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.zone_load_sensible</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.zone_load_latent</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.feb_mean_cop</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.feb_mean_idb</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.feb_mean_humidity_ratio</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.feb_max_cop</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.feb_max_idb</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.feb_max_humidity_ratio</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.feb_min_cop</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.feb_min_idb</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.feb_min_humidity_ratio</t>
-  </si>
-  <si>
-    <t>BESTEST CE Reporting</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.ann_sum_evap_coil_load_total</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.ann_sum_evap_coil_load_sensible</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.ann_sum_evap_coil_load_latent</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.ann_mean_cop2</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.ann_mean_idb</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.ann_mean_zone_relative_humidity_ratio</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.ann_mean_odb</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.ann_mean_outdoor_humidity_ratio</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.may_sept_sum_clg_consumption_total</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.may_sept_sum_clg_consumption_compressor</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.may_sept_sum_clg_consumption_cond_fan</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.may_sept_sum_clg_consumption_indoor_fan</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.may_sept_sum_evap_coil_load_total</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.may_sept_sum_evap_coil_load_sensible</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.may_sept_sum_evap_coil_load_latent</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.may_sept_mean_cop2</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.may_sept_mean_idb</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.may_sept_mean_zone_relative_humidity_ratio</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.energy_consumption_comp_both_fans_wh</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.energy_consumption_comp_both_fans_date</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.energy_consumption_comp_both_fans_hr</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.evap_coil_load_sensible_wh</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.evap_coil_load_sensible_date</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.evap_coil_load_sensible_hr</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.evap_coil_load_latent_wh</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.evap_coil_load_latent_date</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.evap_coil_load_latent_hr</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.evap_coil_load_sensible_and_latent_wh</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.evap_coil_load_sensible_and_latent_date</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.evap_coil_load_sensible_and_latent_hr</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.weather_odb_c</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.weather_odb_date</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.weather_odb_hr</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.weather_outdoor_humidity_ratio_c</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.weather_outdoor_humidity_ratio_date</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.weather_outdoor_humidity_ratio_hr</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.cop2_max_cop2</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.cop2_max_date</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.cop2_max_hr</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.cop2_min_cop2</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.cop2_min_date</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.cop2_min_hr</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.idb_max_idb</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.idb_max_date</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.idb_max_hr</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.idb_min_idb</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.idb_min_date</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.idb_min_hr</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.hr_max_humidity_ratio</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.hr_max_date</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.hr_max_hr</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.hr_min_humidity_ratio</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.hr_min_date</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.hr_min_hr</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.rh_max_relative_humidity</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.rh_max_date</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.rh_max_hr</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.rh_min_relative_humidity</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.rh_min_date</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.rh_min_hr</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0628_hourly_energy_consumpton_compressor</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0628_hourly_energy_consumpton_cond_fan</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0628_hourly_evaporator_coil_load_total</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0628_hourly_evaporator_coil_load_sensible</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0628_hourly_evaporator_coil_load_latent</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0628_hourly_zone_humidity_ratio</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0628_hourly_cop2</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0628_hourly_odb</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0628_hourly_edb</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0628_hourly_ewb</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0628_hourly_outdoor_humidity_ratio</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0430_day_energy_consumption_total</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0430_day_energy_consumption_compressor</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0430_day_energy_consumption_supply_fan</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0430_day_energy_consumption_condenser_fan</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0430_day_evaporator_coil_load_total</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0430_day_evaporator_coil_load_sensible</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0430_day_evaporator_coil_load_latent</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0430_day_zone_humidity_ratio</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0430_day_cop2</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0430_day_odb</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0430_day_edb</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0625_day_energy_consumption_total</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0625_day_energy_consumption_compressor</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0625_day_energy_consumption_supply_fan</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0625_day_energy_consumption_condenser_fan</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0625_day_evaporator_coil_load_total</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0625_day_evaporator_coil_load_sensible</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0625_day_evaporator_coil_load_latent</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0625_day_zone_humidity_ratio</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0625_day_cop2</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0625_day_odb</t>
-  </si>
-  <si>
-    <t>bestest_ce_reporting.0625_day_edb</t>
-  </si>
-  <si>
-    <t>BESTEST Cooling 060812c (fix registerValue name)</t>
+    <t>bestest_ce_reporting.ann_sum_clg_energy_consumption_total</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_sum_clg_energy_consumption_compressor</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_sum_clg_energy_consumption_supply_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_sum_clg_energy_consumption_condenser_fan</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_mean_zone_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.ann_mean_zone_relative_humidity</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_mean_zone_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.may_sept_mean_zone_relative_humidity</t>
+  </si>
+  <si>
+    <t>BESTEST Cooling 060813d (fixed variables)</t>
   </si>
 </sst>
 </file>
@@ -2747,8 +2765,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1589">
+  <cellStyleXfs count="1597">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4440,7 +4466,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1589">
+  <cellStyles count="1597">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5235,6 +5261,10 @@
     <cellStyle name="Followed Hyperlink" xfId="1584" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1586" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1596" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6029,6 +6059,10 @@
     <cellStyle name="Hyperlink" xfId="1583" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1585" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1595" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6502,7 +6536,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>838</v>
+        <v>844</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>470</v>
@@ -6960,7 +6994,7 @@
   <dimension ref="A1:Z53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7144,13 +7178,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>721</v>
+      </c>
+      <c r="D4" s="36" t="s">
         <v>720</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>722</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>721</v>
       </c>
       <c r="E4" s="36" t="s">
         <v>67</v>
@@ -7195,26 +7229,26 @@
       </c>
       <c r="H5" s="37"/>
       <c r="I5" s="37" t="s">
+        <v>717</v>
+      </c>
+      <c r="J5" s="37" t="s">
         <v>718</v>
       </c>
-      <c r="J5" s="37" t="s">
-        <v>719</v>
-      </c>
       <c r="K5" s="37" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="L5" s="37" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="M5" s="37" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="N5" s="37" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="O5" s="41"/>
       <c r="P5" s="43" t="s">
-        <v>717</v>
+        <v>835</v>
       </c>
       <c r="Q5" s="41"/>
       <c r="R5" s="37" t="s">
@@ -7234,13 +7268,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E6" s="36" t="s">
         <v>232</v>
@@ -8600,11 +8634,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M122"/>
+  <dimension ref="A1:M128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C122" sqref="C122"/>
+      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8942,7 +8976,7 @@
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
@@ -8965,7 +8999,7 @@
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -8988,7 +9022,7 @@
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -9011,7 +9045,7 @@
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -9034,7 +9068,7 @@
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -9057,7 +9091,7 @@
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -9080,7 +9114,7 @@
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -9103,7 +9137,7 @@
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -9126,7 +9160,7 @@
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -9149,7 +9183,7 @@
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -9172,7 +9206,7 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -9195,7 +9229,7 @@
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -9218,7 +9252,7 @@
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -9241,7 +9275,7 @@
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -9262,7 +9296,7 @@
     <row r="25" spans="1:13">
       <c r="B25" s="21"/>
       <c r="D25" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="G25" s="15" t="b">
         <v>1</v>
@@ -9277,7 +9311,7 @@
     <row r="26" spans="1:13">
       <c r="B26" s="21"/>
       <c r="D26" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="G26" s="15" t="b">
         <v>1</v>
@@ -9292,7 +9326,7 @@
     <row r="27" spans="1:13">
       <c r="B27" s="21"/>
       <c r="D27" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="G27" s="15" t="b">
         <v>1</v>
@@ -9307,7 +9341,7 @@
     <row r="28" spans="1:13">
       <c r="B28" s="21"/>
       <c r="D28" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="G28" s="15" t="b">
         <v>1</v>
@@ -9322,7 +9356,7 @@
     <row r="29" spans="1:13">
       <c r="B29" s="21"/>
       <c r="D29" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="G29" s="15" t="b">
         <v>1</v>
@@ -9335,10 +9369,10 @@
       </c>
       <c r="J29" s="46"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" s="22" customFormat="1">
       <c r="B30" s="21"/>
-      <c r="D30" s="1" t="s">
-        <v>745</v>
+      <c r="D30" s="15" t="s">
+        <v>836</v>
       </c>
       <c r="G30" s="15" t="b">
         <v>1</v>
@@ -9349,11 +9383,12 @@
       <c r="I30" s="15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="J30" s="46"/>
+    </row>
+    <row r="31" spans="1:13" s="22" customFormat="1">
       <c r="B31" s="21"/>
-      <c r="D31" s="1" t="s">
-        <v>746</v>
+      <c r="D31" s="15" t="s">
+        <v>837</v>
       </c>
       <c r="G31" s="15" t="b">
         <v>1</v>
@@ -9364,11 +9399,12 @@
       <c r="I31" s="15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="J31" s="46"/>
+    </row>
+    <row r="32" spans="1:13" s="22" customFormat="1">
       <c r="B32" s="21"/>
-      <c r="D32" s="1" t="s">
-        <v>747</v>
+      <c r="D32" s="15" t="s">
+        <v>838</v>
       </c>
       <c r="G32" s="15" t="b">
         <v>1</v>
@@ -9379,11 +9415,12 @@
       <c r="I32" s="15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="2:9">
+      <c r="J32" s="46"/>
+    </row>
+    <row r="33" spans="2:10" s="22" customFormat="1">
       <c r="B33" s="21"/>
-      <c r="D33" s="1" t="s">
-        <v>748</v>
+      <c r="D33" s="15" t="s">
+        <v>839</v>
       </c>
       <c r="G33" s="15" t="b">
         <v>1</v>
@@ -9394,11 +9431,12 @@
       <c r="I33" s="15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:9">
+      <c r="J33" s="46"/>
+    </row>
+    <row r="34" spans="2:10">
       <c r="B34" s="21"/>
       <c r="D34" s="1" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="G34" s="15" t="b">
         <v>1</v>
@@ -9410,10 +9448,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:10">
       <c r="B35" s="21"/>
       <c r="D35" s="1" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="G35" s="15" t="b">
         <v>1</v>
@@ -9425,10 +9463,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:10">
       <c r="B36" s="21"/>
       <c r="D36" s="1" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="G36" s="15" t="b">
         <v>1</v>
@@ -9440,10 +9478,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:10">
       <c r="B37" s="21"/>
       <c r="D37" s="1" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="G37" s="15" t="b">
         <v>1</v>
@@ -9455,10 +9493,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="2:10">
       <c r="B38" s="21"/>
       <c r="D38" s="1" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
       <c r="G38" s="15" t="b">
         <v>1</v>
@@ -9470,10 +9508,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:10" s="22" customFormat="1">
       <c r="B39" s="21"/>
-      <c r="D39" s="1" t="s">
-        <v>754</v>
+      <c r="D39" s="22" t="s">
+        <v>840</v>
       </c>
       <c r="G39" s="15" t="b">
         <v>1</v>
@@ -9485,10 +9523,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:10">
       <c r="B40" s="21"/>
       <c r="D40" s="1" t="s">
-        <v>755</v>
+        <v>841</v>
       </c>
       <c r="G40" s="15" t="b">
         <v>1</v>
@@ -9500,10 +9538,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="2:10">
       <c r="B41" s="21"/>
       <c r="D41" s="1" t="s">
-        <v>756</v>
+        <v>749</v>
       </c>
       <c r="G41" s="15" t="b">
         <v>1</v>
@@ -9515,10 +9553,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:9">
+    <row r="42" spans="2:10">
       <c r="B42" s="21"/>
       <c r="D42" s="1" t="s">
-        <v>757</v>
+        <v>750</v>
       </c>
       <c r="G42" s="15" t="b">
         <v>1</v>
@@ -9530,10 +9568,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:9">
+    <row r="43" spans="2:10">
       <c r="B43" s="21"/>
       <c r="D43" s="1" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
       <c r="G43" s="15" t="b">
         <v>1</v>
@@ -9545,10 +9583,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:9">
+    <row r="44" spans="2:10">
       <c r="B44" s="21"/>
       <c r="D44" s="1" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
       <c r="G44" s="15" t="b">
         <v>1</v>
@@ -9560,10 +9598,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:9">
+    <row r="45" spans="2:10">
       <c r="B45" s="21"/>
       <c r="D45" s="1" t="s">
-        <v>760</v>
+        <v>753</v>
       </c>
       <c r="G45" s="15" t="b">
         <v>1</v>
@@ -9575,10 +9613,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:9">
+    <row r="46" spans="2:10">
       <c r="B46" s="21"/>
       <c r="D46" s="1" t="s">
-        <v>761</v>
+        <v>754</v>
       </c>
       <c r="G46" s="15" t="b">
         <v>1</v>
@@ -9590,10 +9628,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:9">
+    <row r="47" spans="2:10">
       <c r="B47" s="21"/>
       <c r="D47" s="1" t="s">
-        <v>762</v>
+        <v>755</v>
       </c>
       <c r="G47" s="15" t="b">
         <v>1</v>
@@ -9605,10 +9643,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:9">
+    <row r="48" spans="2:10">
       <c r="B48" s="21"/>
       <c r="D48" s="1" t="s">
-        <v>763</v>
+        <v>756</v>
       </c>
       <c r="G48" s="15" t="b">
         <v>1</v>
@@ -9623,7 +9661,7 @@
     <row r="49" spans="2:9">
       <c r="B49" s="21"/>
       <c r="D49" s="1" t="s">
-        <v>764</v>
+        <v>757</v>
       </c>
       <c r="G49" s="15" t="b">
         <v>1</v>
@@ -9638,7 +9676,7 @@
     <row r="50" spans="2:9">
       <c r="B50" s="21"/>
       <c r="D50" s="1" t="s">
-        <v>765</v>
+        <v>758</v>
       </c>
       <c r="G50" s="15" t="b">
         <v>1</v>
@@ -9653,7 +9691,7 @@
     <row r="51" spans="2:9">
       <c r="B51" s="21"/>
       <c r="D51" s="1" t="s">
-        <v>766</v>
+        <v>759</v>
       </c>
       <c r="G51" s="15" t="b">
         <v>1</v>
@@ -9665,10 +9703,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="2:9" s="22" customFormat="1">
       <c r="B52" s="21"/>
-      <c r="D52" s="1" t="s">
-        <v>767</v>
+      <c r="D52" s="22" t="s">
+        <v>842</v>
       </c>
       <c r="G52" s="15" t="b">
         <v>1</v>
@@ -9683,7 +9721,7 @@
     <row r="53" spans="2:9">
       <c r="B53" s="21"/>
       <c r="D53" s="1" t="s">
-        <v>768</v>
+        <v>843</v>
       </c>
       <c r="G53" s="15" t="b">
         <v>1</v>
@@ -9698,7 +9736,7 @@
     <row r="54" spans="2:9">
       <c r="B54" s="21"/>
       <c r="D54" s="1" t="s">
-        <v>769</v>
+        <v>760</v>
       </c>
       <c r="G54" s="15" t="b">
         <v>1</v>
@@ -9713,7 +9751,7 @@
     <row r="55" spans="2:9">
       <c r="B55" s="21"/>
       <c r="D55" s="1" t="s">
-        <v>770</v>
+        <v>761</v>
       </c>
       <c r="G55" s="15" t="b">
         <v>1</v>
@@ -9728,7 +9766,7 @@
     <row r="56" spans="2:9">
       <c r="B56" s="21"/>
       <c r="D56" s="1" t="s">
-        <v>771</v>
+        <v>762</v>
       </c>
       <c r="G56" s="15" t="b">
         <v>1</v>
@@ -9743,7 +9781,7 @@
     <row r="57" spans="2:9">
       <c r="B57" s="21"/>
       <c r="D57" s="1" t="s">
-        <v>772</v>
+        <v>763</v>
       </c>
       <c r="G57" s="15" t="b">
         <v>1</v>
@@ -9758,7 +9796,7 @@
     <row r="58" spans="2:9">
       <c r="B58" s="21"/>
       <c r="D58" s="1" t="s">
-        <v>773</v>
+        <v>764</v>
       </c>
       <c r="G58" s="15" t="b">
         <v>1</v>
@@ -9773,7 +9811,7 @@
     <row r="59" spans="2:9">
       <c r="B59" s="21"/>
       <c r="D59" s="1" t="s">
-        <v>774</v>
+        <v>765</v>
       </c>
       <c r="G59" s="15" t="b">
         <v>1</v>
@@ -9788,7 +9826,7 @@
     <row r="60" spans="2:9">
       <c r="B60" s="21"/>
       <c r="D60" s="1" t="s">
-        <v>775</v>
+        <v>766</v>
       </c>
       <c r="G60" s="15" t="b">
         <v>1</v>
@@ -9803,7 +9841,7 @@
     <row r="61" spans="2:9">
       <c r="B61" s="21"/>
       <c r="D61" s="1" t="s">
-        <v>776</v>
+        <v>767</v>
       </c>
       <c r="G61" s="15" t="b">
         <v>1</v>
@@ -9818,7 +9856,7 @@
     <row r="62" spans="2:9">
       <c r="B62" s="21"/>
       <c r="D62" s="1" t="s">
-        <v>777</v>
+        <v>768</v>
       </c>
       <c r="G62" s="15" t="b">
         <v>1</v>
@@ -9833,7 +9871,7 @@
     <row r="63" spans="2:9">
       <c r="B63" s="21"/>
       <c r="D63" s="1" t="s">
-        <v>778</v>
+        <v>769</v>
       </c>
       <c r="G63" s="15" t="b">
         <v>1</v>
@@ -9848,7 +9886,7 @@
     <row r="64" spans="2:9">
       <c r="B64" s="21"/>
       <c r="D64" s="1" t="s">
-        <v>779</v>
+        <v>770</v>
       </c>
       <c r="G64" s="15" t="b">
         <v>1</v>
@@ -9863,7 +9901,7 @@
     <row r="65" spans="2:9">
       <c r="B65" s="21"/>
       <c r="D65" s="1" t="s">
-        <v>780</v>
+        <v>771</v>
       </c>
       <c r="G65" s="15" t="b">
         <v>1</v>
@@ -9878,7 +9916,7 @@
     <row r="66" spans="2:9">
       <c r="B66" s="21"/>
       <c r="D66" s="1" t="s">
-        <v>781</v>
+        <v>772</v>
       </c>
       <c r="G66" s="15" t="b">
         <v>1</v>
@@ -9893,7 +9931,7 @@
     <row r="67" spans="2:9">
       <c r="B67" s="21"/>
       <c r="D67" s="1" t="s">
-        <v>782</v>
+        <v>773</v>
       </c>
       <c r="G67" s="15" t="b">
         <v>1</v>
@@ -9908,7 +9946,7 @@
     <row r="68" spans="2:9">
       <c r="B68" s="21"/>
       <c r="D68" s="1" t="s">
-        <v>783</v>
+        <v>774</v>
       </c>
       <c r="G68" s="15" t="b">
         <v>1</v>
@@ -9923,7 +9961,7 @@
     <row r="69" spans="2:9">
       <c r="B69" s="21"/>
       <c r="D69" s="1" t="s">
-        <v>784</v>
+        <v>775</v>
       </c>
       <c r="G69" s="15" t="b">
         <v>1</v>
@@ -9938,7 +9976,7 @@
     <row r="70" spans="2:9">
       <c r="B70" s="21"/>
       <c r="D70" s="1" t="s">
-        <v>785</v>
+        <v>776</v>
       </c>
       <c r="G70" s="15" t="b">
         <v>1</v>
@@ -9953,7 +9991,7 @@
     <row r="71" spans="2:9">
       <c r="B71" s="21"/>
       <c r="D71" s="1" t="s">
-        <v>786</v>
+        <v>777</v>
       </c>
       <c r="G71" s="15" t="b">
         <v>1</v>
@@ -9968,7 +10006,7 @@
     <row r="72" spans="2:9">
       <c r="B72" s="21"/>
       <c r="D72" s="1" t="s">
-        <v>787</v>
+        <v>778</v>
       </c>
       <c r="G72" s="15" t="b">
         <v>1</v>
@@ -9983,7 +10021,7 @@
     <row r="73" spans="2:9">
       <c r="B73" s="21"/>
       <c r="D73" s="1" t="s">
-        <v>788</v>
+        <v>779</v>
       </c>
       <c r="G73" s="15" t="b">
         <v>1</v>
@@ -9998,7 +10036,7 @@
     <row r="74" spans="2:9">
       <c r="B74" s="21"/>
       <c r="D74" s="1" t="s">
-        <v>789</v>
+        <v>780</v>
       </c>
       <c r="G74" s="15" t="b">
         <v>1</v>
@@ -10013,7 +10051,7 @@
     <row r="75" spans="2:9">
       <c r="B75" s="21"/>
       <c r="D75" s="1" t="s">
-        <v>790</v>
+        <v>781</v>
       </c>
       <c r="G75" s="15" t="b">
         <v>1</v>
@@ -10028,7 +10066,7 @@
     <row r="76" spans="2:9">
       <c r="B76" s="21"/>
       <c r="D76" s="1" t="s">
-        <v>791</v>
+        <v>782</v>
       </c>
       <c r="G76" s="15" t="b">
         <v>1</v>
@@ -10043,7 +10081,7 @@
     <row r="77" spans="2:9">
       <c r="B77" s="21"/>
       <c r="D77" s="1" t="s">
-        <v>792</v>
+        <v>783</v>
       </c>
       <c r="G77" s="15" t="b">
         <v>1</v>
@@ -10058,7 +10096,7 @@
     <row r="78" spans="2:9">
       <c r="B78" s="21"/>
       <c r="D78" s="1" t="s">
-        <v>793</v>
+        <v>784</v>
       </c>
       <c r="G78" s="15" t="b">
         <v>1</v>
@@ -10073,7 +10111,7 @@
     <row r="79" spans="2:9">
       <c r="B79" s="21"/>
       <c r="D79" s="1" t="s">
-        <v>794</v>
+        <v>785</v>
       </c>
       <c r="G79" s="15" t="b">
         <v>1</v>
@@ -10088,7 +10126,7 @@
     <row r="80" spans="2:9">
       <c r="B80" s="21"/>
       <c r="D80" s="1" t="s">
-        <v>795</v>
+        <v>786</v>
       </c>
       <c r="G80" s="15" t="b">
         <v>1</v>
@@ -10103,7 +10141,7 @@
     <row r="81" spans="2:9">
       <c r="B81" s="21"/>
       <c r="D81" s="1" t="s">
-        <v>796</v>
+        <v>787</v>
       </c>
       <c r="G81" s="15" t="b">
         <v>1</v>
@@ -10118,7 +10156,7 @@
     <row r="82" spans="2:9">
       <c r="B82" s="21"/>
       <c r="D82" s="1" t="s">
-        <v>797</v>
+        <v>788</v>
       </c>
       <c r="G82" s="15" t="b">
         <v>1</v>
@@ -10133,7 +10171,7 @@
     <row r="83" spans="2:9">
       <c r="B83" s="21"/>
       <c r="D83" s="1" t="s">
-        <v>798</v>
+        <v>789</v>
       </c>
       <c r="G83" s="15" t="b">
         <v>1</v>
@@ -10148,7 +10186,7 @@
     <row r="84" spans="2:9">
       <c r="B84" s="21"/>
       <c r="D84" s="1" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
       <c r="G84" s="15" t="b">
         <v>1</v>
@@ -10163,7 +10201,7 @@
     <row r="85" spans="2:9">
       <c r="B85" s="21"/>
       <c r="D85" s="1" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
       <c r="G85" s="15" t="b">
         <v>1</v>
@@ -10178,7 +10216,7 @@
     <row r="86" spans="2:9">
       <c r="B86" s="21"/>
       <c r="D86" s="1" t="s">
-        <v>801</v>
+        <v>792</v>
       </c>
       <c r="G86" s="15" t="b">
         <v>1</v>
@@ -10193,7 +10231,7 @@
     <row r="87" spans="2:9">
       <c r="B87" s="21"/>
       <c r="D87" s="1" t="s">
-        <v>802</v>
+        <v>793</v>
       </c>
       <c r="G87" s="15" t="b">
         <v>1</v>
@@ -10208,7 +10246,7 @@
     <row r="88" spans="2:9">
       <c r="B88" s="21"/>
       <c r="D88" s="1" t="s">
-        <v>803</v>
+        <v>794</v>
       </c>
       <c r="G88" s="15" t="b">
         <v>1</v>
@@ -10223,7 +10261,7 @@
     <row r="89" spans="2:9">
       <c r="B89" s="21"/>
       <c r="D89" s="1" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
       <c r="G89" s="15" t="b">
         <v>1</v>
@@ -10238,7 +10276,7 @@
     <row r="90" spans="2:9">
       <c r="B90" s="21"/>
       <c r="D90" s="1" t="s">
-        <v>805</v>
+        <v>796</v>
       </c>
       <c r="G90" s="15" t="b">
         <v>1</v>
@@ -10251,8 +10289,9 @@
       </c>
     </row>
     <row r="91" spans="2:9">
+      <c r="B91" s="21"/>
       <c r="D91" s="1" t="s">
-        <v>806</v>
+        <v>797</v>
       </c>
       <c r="G91" s="15" t="b">
         <v>1</v>
@@ -10265,8 +10304,9 @@
       </c>
     </row>
     <row r="92" spans="2:9">
+      <c r="B92" s="21"/>
       <c r="D92" s="1" t="s">
-        <v>807</v>
+        <v>798</v>
       </c>
       <c r="G92" s="15" t="b">
         <v>1</v>
@@ -10279,8 +10319,9 @@
       </c>
     </row>
     <row r="93" spans="2:9">
+      <c r="B93" s="21"/>
       <c r="D93" s="1" t="s">
-        <v>808</v>
+        <v>799</v>
       </c>
       <c r="G93" s="15" t="b">
         <v>1</v>
@@ -10293,8 +10334,9 @@
       </c>
     </row>
     <row r="94" spans="2:9">
+      <c r="B94" s="21"/>
       <c r="D94" s="1" t="s">
-        <v>809</v>
+        <v>800</v>
       </c>
       <c r="G94" s="15" t="b">
         <v>1</v>
@@ -10307,8 +10349,9 @@
       </c>
     </row>
     <row r="95" spans="2:9">
+      <c r="B95" s="21"/>
       <c r="D95" s="1" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="G95" s="15" t="b">
         <v>1</v>
@@ -10321,8 +10364,9 @@
       </c>
     </row>
     <row r="96" spans="2:9">
+      <c r="B96" s="21"/>
       <c r="D96" s="1" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="G96" s="15" t="b">
         <v>1</v>
@@ -10336,7 +10380,7 @@
     </row>
     <row r="97" spans="4:9">
       <c r="D97" s="1" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="G97" s="15" t="b">
         <v>1</v>
@@ -10350,7 +10394,7 @@
     </row>
     <row r="98" spans="4:9">
       <c r="D98" s="1" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="G98" s="15" t="b">
         <v>1</v>
@@ -10364,7 +10408,7 @@
     </row>
     <row r="99" spans="4:9">
       <c r="D99" s="1" t="s">
-        <v>814</v>
+        <v>805</v>
       </c>
       <c r="G99" s="15" t="b">
         <v>1</v>
@@ -10378,7 +10422,7 @@
     </row>
     <row r="100" spans="4:9">
       <c r="D100" s="1" t="s">
-        <v>815</v>
+        <v>806</v>
       </c>
       <c r="G100" s="15" t="b">
         <v>1</v>
@@ -10392,7 +10436,7 @@
     </row>
     <row r="101" spans="4:9">
       <c r="D101" s="1" t="s">
-        <v>816</v>
+        <v>807</v>
       </c>
       <c r="G101" s="15" t="b">
         <v>1</v>
@@ -10406,7 +10450,7 @@
     </row>
     <row r="102" spans="4:9">
       <c r="D102" s="1" t="s">
-        <v>817</v>
+        <v>808</v>
       </c>
       <c r="G102" s="15" t="b">
         <v>1</v>
@@ -10420,7 +10464,7 @@
     </row>
     <row r="103" spans="4:9">
       <c r="D103" s="1" t="s">
-        <v>818</v>
+        <v>809</v>
       </c>
       <c r="G103" s="15" t="b">
         <v>1</v>
@@ -10434,7 +10478,7 @@
     </row>
     <row r="104" spans="4:9">
       <c r="D104" s="1" t="s">
-        <v>819</v>
+        <v>810</v>
       </c>
       <c r="G104" s="15" t="b">
         <v>1</v>
@@ -10448,7 +10492,7 @@
     </row>
     <row r="105" spans="4:9">
       <c r="D105" s="1" t="s">
-        <v>820</v>
+        <v>811</v>
       </c>
       <c r="G105" s="15" t="b">
         <v>1</v>
@@ -10462,7 +10506,7 @@
     </row>
     <row r="106" spans="4:9">
       <c r="D106" s="1" t="s">
-        <v>821</v>
+        <v>812</v>
       </c>
       <c r="G106" s="15" t="b">
         <v>1</v>
@@ -10476,7 +10520,7 @@
     </row>
     <row r="107" spans="4:9">
       <c r="D107" s="1" t="s">
-        <v>822</v>
+        <v>813</v>
       </c>
       <c r="G107" s="15" t="b">
         <v>1</v>
@@ -10490,7 +10534,7 @@
     </row>
     <row r="108" spans="4:9">
       <c r="D108" s="1" t="s">
-        <v>823</v>
+        <v>814</v>
       </c>
       <c r="G108" s="15" t="b">
         <v>1</v>
@@ -10504,7 +10548,7 @@
     </row>
     <row r="109" spans="4:9">
       <c r="D109" s="1" t="s">
-        <v>824</v>
+        <v>815</v>
       </c>
       <c r="G109" s="15" t="b">
         <v>1</v>
@@ -10518,7 +10562,7 @@
     </row>
     <row r="110" spans="4:9">
       <c r="D110" s="1" t="s">
-        <v>825</v>
+        <v>816</v>
       </c>
       <c r="G110" s="15" t="b">
         <v>1</v>
@@ -10532,7 +10576,7 @@
     </row>
     <row r="111" spans="4:9">
       <c r="D111" s="1" t="s">
-        <v>826</v>
+        <v>817</v>
       </c>
       <c r="G111" s="15" t="b">
         <v>1</v>
@@ -10546,7 +10590,7 @@
     </row>
     <row r="112" spans="4:9">
       <c r="D112" s="1" t="s">
-        <v>827</v>
+        <v>818</v>
       </c>
       <c r="G112" s="15" t="b">
         <v>1</v>
@@ -10560,7 +10604,7 @@
     </row>
     <row r="113" spans="4:9">
       <c r="D113" s="1" t="s">
-        <v>828</v>
+        <v>819</v>
       </c>
       <c r="G113" s="15" t="b">
         <v>1</v>
@@ -10574,7 +10618,7 @@
     </row>
     <row r="114" spans="4:9">
       <c r="D114" s="1" t="s">
-        <v>829</v>
+        <v>820</v>
       </c>
       <c r="G114" s="15" t="b">
         <v>1</v>
@@ -10588,7 +10632,7 @@
     </row>
     <row r="115" spans="4:9">
       <c r="D115" s="1" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
       <c r="G115" s="15" t="b">
         <v>1</v>
@@ -10602,7 +10646,7 @@
     </row>
     <row r="116" spans="4:9">
       <c r="D116" s="1" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
       <c r="G116" s="15" t="b">
         <v>1</v>
@@ -10616,7 +10660,7 @@
     </row>
     <row r="117" spans="4:9">
       <c r="D117" s="1" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="G117" s="15" t="b">
         <v>1</v>
@@ -10630,7 +10674,7 @@
     </row>
     <row r="118" spans="4:9">
       <c r="D118" s="1" t="s">
-        <v>833</v>
+        <v>824</v>
       </c>
       <c r="G118" s="15" t="b">
         <v>1</v>
@@ -10644,7 +10688,7 @@
     </row>
     <row r="119" spans="4:9">
       <c r="D119" s="1" t="s">
-        <v>834</v>
+        <v>825</v>
       </c>
       <c r="G119" s="15" t="b">
         <v>1</v>
@@ -10658,7 +10702,7 @@
     </row>
     <row r="120" spans="4:9">
       <c r="D120" s="1" t="s">
-        <v>835</v>
+        <v>826</v>
       </c>
       <c r="G120" s="15" t="b">
         <v>1</v>
@@ -10672,7 +10716,7 @@
     </row>
     <row r="121" spans="4:9">
       <c r="D121" s="1" t="s">
-        <v>836</v>
+        <v>827</v>
       </c>
       <c r="G121" s="15" t="b">
         <v>1</v>
@@ -10686,7 +10730,7 @@
     </row>
     <row r="122" spans="4:9">
       <c r="D122" s="1" t="s">
-        <v>837</v>
+        <v>828</v>
       </c>
       <c r="G122" s="15" t="b">
         <v>1</v>
@@ -10695,6 +10739,90 @@
         <v>1</v>
       </c>
       <c r="I122" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="4:9">
+      <c r="D123" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="G123" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H123" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I123" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="4:9">
+      <c r="D124" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="G124" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H124" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I124" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="4:9">
+      <c r="D125" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="G125" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H125" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I125" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="4:9">
+      <c r="D126" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="G126" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H126" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I126" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="4:9">
+      <c r="D127" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="G127" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H127" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I127" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="4:9">
+      <c r="D128" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="G128" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H128" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I128" s="15" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
populated sum and mean table for 5-3B
Still need to address may-sept for 500 and 510
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20460" tabRatio="562"/>
@@ -2575,7 +2575,7 @@
     <t>bestest_ce_reporting.may_sept_mean_zone_relative_humidity</t>
   </si>
   <si>
-    <t>BESTEST Cooling 060813d (fixed variables)</t>
+    <t>BESTEST Cooling 061026a (adding avg sums and means)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
5-3B min/max table with date and hour
Need to go back and add April-Dec values for 5xx cases
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20460" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="41460" windowHeight="26540" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2281" uniqueCount="869">
   <si>
     <t>type</t>
   </si>
@@ -2575,7 +2575,79 @@
     <t>bestest_ce_reporting.may_sept_mean_zone_relative_humidity</t>
   </si>
   <si>
-    <t>BESTEST Cooling 061026b (adding max table)</t>
+    <t>bestest_ce_reporting.apr_dec_cop2_max_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_cop2_max_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_cop2_max_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_cop2_min_cop2</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_cop2_min_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_cop2_min_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_idb_max_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_idb_max_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_idb_max_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_idb_min_idb</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_idb_min_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_idb_min_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_hr_max_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_hr_max_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_hr_max_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_hr_min_humidity_ratio</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_hr_min_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_hr_min_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_rh_max_relative_humidity</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_rh_max_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_rh_max_hr</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_rh_min_relative_humidity</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_rh_min_date</t>
+  </si>
+  <si>
+    <t>bestest_ce_reporting.apr_dec_rh_min_hr</t>
+  </si>
+  <si>
+    <t>BESTEST Cooling 061026d (extending outputs for apr_dec)</t>
   </si>
 </sst>
 </file>
@@ -2765,8 +2837,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1597">
+  <cellStyleXfs count="1599">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4466,7 +4540,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1597">
+  <cellStyles count="1599">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5265,6 +5339,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1592" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1594" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1598" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6063,6 +6138,7 @@
     <cellStyle name="Hyperlink" xfId="1591" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1593" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1597" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6536,7 +6612,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>844</v>
+        <v>868</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>470</v>
@@ -8634,11 +8710,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M128"/>
+  <dimension ref="A1:M152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <pane ySplit="3" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A96" sqref="A96:XFD119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10363,466 +10439,826 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:9">
+    <row r="96" spans="2:9" s="22" customFormat="1">
       <c r="B96" s="21"/>
-      <c r="D96" s="1" t="s">
+      <c r="D96" s="22" t="s">
+        <v>844</v>
+      </c>
+      <c r="G96" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H96" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I96" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" s="22" customFormat="1">
+      <c r="B97" s="21"/>
+      <c r="D97" s="22" t="s">
+        <v>845</v>
+      </c>
+      <c r="G97" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H97" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I97" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" s="22" customFormat="1">
+      <c r="B98" s="21"/>
+      <c r="D98" s="22" t="s">
+        <v>846</v>
+      </c>
+      <c r="G98" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H98" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I98" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" s="22" customFormat="1">
+      <c r="B99" s="21"/>
+      <c r="D99" s="22" t="s">
+        <v>847</v>
+      </c>
+      <c r="G99" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H99" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I99" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" s="22" customFormat="1">
+      <c r="B100" s="21"/>
+      <c r="D100" s="22" t="s">
+        <v>848</v>
+      </c>
+      <c r="G100" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H100" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I100" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" s="22" customFormat="1">
+      <c r="B101" s="21"/>
+      <c r="D101" s="22" t="s">
+        <v>849</v>
+      </c>
+      <c r="G101" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H101" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I101" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" s="22" customFormat="1">
+      <c r="B102" s="21"/>
+      <c r="D102" s="22" t="s">
+        <v>850</v>
+      </c>
+      <c r="G102" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H102" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I102" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" s="22" customFormat="1">
+      <c r="B103" s="21"/>
+      <c r="D103" s="22" t="s">
+        <v>851</v>
+      </c>
+      <c r="G103" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H103" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I103" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" s="22" customFormat="1">
+      <c r="B104" s="21"/>
+      <c r="D104" s="22" t="s">
+        <v>852</v>
+      </c>
+      <c r="G104" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H104" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I104" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" s="22" customFormat="1">
+      <c r="B105" s="21"/>
+      <c r="D105" s="22" t="s">
+        <v>853</v>
+      </c>
+      <c r="G105" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H105" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I105" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" s="22" customFormat="1">
+      <c r="B106" s="21"/>
+      <c r="D106" s="22" t="s">
+        <v>854</v>
+      </c>
+      <c r="G106" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H106" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I106" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" s="22" customFormat="1">
+      <c r="B107" s="21"/>
+      <c r="D107" s="22" t="s">
+        <v>855</v>
+      </c>
+      <c r="G107" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H107" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I107" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" s="22" customFormat="1">
+      <c r="B108" s="21"/>
+      <c r="D108" s="22" t="s">
+        <v>856</v>
+      </c>
+      <c r="G108" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H108" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I108" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" s="22" customFormat="1">
+      <c r="B109" s="21"/>
+      <c r="D109" s="22" t="s">
+        <v>857</v>
+      </c>
+      <c r="G109" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H109" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I109" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" s="22" customFormat="1">
+      <c r="B110" s="21"/>
+      <c r="D110" s="22" t="s">
+        <v>858</v>
+      </c>
+      <c r="G110" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H110" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I110" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" s="22" customFormat="1">
+      <c r="B111" s="21"/>
+      <c r="D111" s="22" t="s">
+        <v>859</v>
+      </c>
+      <c r="G111" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H111" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I111" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" s="22" customFormat="1">
+      <c r="B112" s="21"/>
+      <c r="D112" s="22" t="s">
+        <v>860</v>
+      </c>
+      <c r="G112" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H112" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I112" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" s="22" customFormat="1">
+      <c r="B113" s="21"/>
+      <c r="D113" s="22" t="s">
+        <v>861</v>
+      </c>
+      <c r="G113" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H113" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I113" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" s="22" customFormat="1">
+      <c r="B114" s="21"/>
+      <c r="D114" s="22" t="s">
+        <v>862</v>
+      </c>
+      <c r="G114" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H114" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I114" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9" s="22" customFormat="1">
+      <c r="B115" s="21"/>
+      <c r="D115" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="G115" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H115" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I115" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" s="22" customFormat="1">
+      <c r="B116" s="21"/>
+      <c r="D116" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="G116" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H116" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I116" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9" s="22" customFormat="1">
+      <c r="B117" s="21"/>
+      <c r="D117" s="22" t="s">
+        <v>865</v>
+      </c>
+      <c r="G117" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H117" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I117" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="2:9" s="22" customFormat="1">
+      <c r="B118" s="21"/>
+      <c r="D118" s="22" t="s">
+        <v>866</v>
+      </c>
+      <c r="G118" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H118" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I118" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:9" s="22" customFormat="1">
+      <c r="B119" s="21"/>
+      <c r="D119" s="22" t="s">
+        <v>867</v>
+      </c>
+      <c r="G119" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H119" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I119" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9">
+      <c r="B120" s="21"/>
+      <c r="D120" s="1" t="s">
         <v>802</v>
       </c>
-      <c r="G96" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H96" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I96" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="4:9">
-      <c r="D97" s="1" t="s">
+      <c r="G120" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H120" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I120" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9">
+      <c r="D121" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="G97" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H97" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I97" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="4:9">
-      <c r="D98" s="1" t="s">
+      <c r="G121" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H121" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I121" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="2:9">
+      <c r="D122" s="1" t="s">
         <v>804</v>
       </c>
-      <c r="G98" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H98" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I98" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="4:9">
-      <c r="D99" s="1" t="s">
+      <c r="G122" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H122" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I122" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="2:9">
+      <c r="D123" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="G99" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H99" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I99" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="4:9">
-      <c r="D100" s="1" t="s">
+      <c r="G123" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H123" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I123" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="2:9">
+      <c r="D124" s="1" t="s">
         <v>806</v>
       </c>
-      <c r="G100" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H100" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I100" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="4:9">
-      <c r="D101" s="1" t="s">
+      <c r="G124" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H124" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I124" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="2:9">
+      <c r="D125" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="G101" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H101" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I101" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="4:9">
-      <c r="D102" s="1" t="s">
+      <c r="G125" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H125" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I125" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="2:9">
+      <c r="D126" s="1" t="s">
         <v>808</v>
       </c>
-      <c r="G102" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H102" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I102" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="4:9">
-      <c r="D103" s="1" t="s">
+      <c r="G126" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H126" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I126" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="2:9">
+      <c r="D127" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="G103" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H103" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I103" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="4:9">
-      <c r="D104" s="1" t="s">
+      <c r="G127" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H127" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I127" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="2:9">
+      <c r="D128" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="G104" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H104" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I104" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="4:9">
-      <c r="D105" s="1" t="s">
+      <c r="G128" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H128" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I128" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="4:9">
+      <c r="D129" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="G105" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H105" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I105" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="4:9">
-      <c r="D106" s="1" t="s">
+      <c r="G129" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H129" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I129" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="4:9">
+      <c r="D130" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="G106" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H106" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I106" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="4:9">
-      <c r="D107" s="1" t="s">
+      <c r="G130" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H130" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I130" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="4:9">
+      <c r="D131" s="1" t="s">
         <v>813</v>
       </c>
-      <c r="G107" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H107" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I107" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="4:9">
-      <c r="D108" s="1" t="s">
+      <c r="G131" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H131" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I131" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="4:9">
+      <c r="D132" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="G108" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H108" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I108" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="4:9">
-      <c r="D109" s="1" t="s">
+      <c r="G132" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H132" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I132" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="4:9">
+      <c r="D133" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="G109" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H109" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I109" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="4:9">
-      <c r="D110" s="1" t="s">
+      <c r="G133" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H133" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I133" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="4:9">
+      <c r="D134" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="G110" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H110" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I110" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="4:9">
-      <c r="D111" s="1" t="s">
+      <c r="G134" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H134" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I134" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="4:9">
+      <c r="D135" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="G111" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H111" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I111" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="4:9">
-      <c r="D112" s="1" t="s">
+      <c r="G135" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H135" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I135" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="4:9">
+      <c r="D136" s="1" t="s">
         <v>818</v>
       </c>
-      <c r="G112" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H112" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I112" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="4:9">
-      <c r="D113" s="1" t="s">
+      <c r="G136" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H136" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I136" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="4:9">
+      <c r="D137" s="1" t="s">
         <v>819</v>
       </c>
-      <c r="G113" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H113" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I113" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="4:9">
-      <c r="D114" s="1" t="s">
+      <c r="G137" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H137" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I137" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="4:9">
+      <c r="D138" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="G114" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H114" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I114" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="4:9">
-      <c r="D115" s="1" t="s">
+      <c r="G138" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H138" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I138" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="4:9">
+      <c r="D139" s="1" t="s">
         <v>821</v>
       </c>
-      <c r="G115" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H115" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I115" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="4:9">
-      <c r="D116" s="1" t="s">
+      <c r="G139" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H139" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I139" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="4:9">
+      <c r="D140" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="G116" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H116" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I116" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="4:9">
-      <c r="D117" s="1" t="s">
+      <c r="G140" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H140" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I140" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="4:9">
+      <c r="D141" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="G117" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H117" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I117" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="4:9">
-      <c r="D118" s="1" t="s">
+      <c r="G141" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H141" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I141" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="4:9">
+      <c r="D142" s="1" t="s">
         <v>824</v>
       </c>
-      <c r="G118" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H118" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I118" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="4:9">
-      <c r="D119" s="1" t="s">
+      <c r="G142" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H142" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I142" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="4:9">
+      <c r="D143" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="G119" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H119" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I119" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="4:9">
-      <c r="D120" s="1" t="s">
+      <c r="G143" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H143" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I143" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="4:9">
+      <c r="D144" s="1" t="s">
         <v>826</v>
       </c>
-      <c r="G120" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H120" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I120" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="4:9">
-      <c r="D121" s="1" t="s">
+      <c r="G144" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H144" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I144" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="4:9">
+      <c r="D145" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="G121" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H121" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I121" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="4:9">
-      <c r="D122" s="1" t="s">
+      <c r="G145" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H145" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I145" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="4:9">
+      <c r="D146" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="G122" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H122" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I122" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="4:9">
-      <c r="D123" s="1" t="s">
+      <c r="G146" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H146" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I146" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="4:9">
+      <c r="D147" s="1" t="s">
         <v>829</v>
       </c>
-      <c r="G123" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H123" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I123" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="4:9">
-      <c r="D124" s="1" t="s">
+      <c r="G147" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H147" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I147" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="4:9">
+      <c r="D148" s="1" t="s">
         <v>830</v>
       </c>
-      <c r="G124" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H124" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I124" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="4:9">
-      <c r="D125" s="1" t="s">
+      <c r="G148" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H148" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I148" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="4:9">
+      <c r="D149" s="1" t="s">
         <v>831</v>
       </c>
-      <c r="G125" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H125" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I125" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="4:9">
-      <c r="D126" s="1" t="s">
+      <c r="G149" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H149" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I149" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="4:9">
+      <c r="D150" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="G126" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H126" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I126" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="4:9">
-      <c r="D127" s="1" t="s">
+      <c r="G150" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H150" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I150" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="4:9">
+      <c r="D151" s="1" t="s">
         <v>833</v>
       </c>
-      <c r="G127" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H127" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I127" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="4:9">
-      <c r="D128" s="1" t="s">
+      <c r="G151" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H151" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I151" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="4:9">
+      <c r="D152" s="1" t="s">
         <v>834</v>
       </c>
-      <c r="G128" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H128" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I128" s="15" t="b">
+      <c r="G152" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H152" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I152" s="15" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Making CExxx fans cycle
Added additional test cases.
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="41460" windowHeight="26540" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="23460" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2647,7 +2647,7 @@
     <t>bestest_ce_reporting.apr_dec_rh_min_hr</t>
   </si>
   <si>
-    <t>BESTEST Cooling 061027a (daily hourly and avg)</t>
+    <t>BESTEST Cooling 061027d (work around for NaN on COP calc)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
populating partial year values
may-sept and apr-dec
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -2647,7 +2647,7 @@
     <t>bestest_ce_reporting.apr_dec_rh_min_hr</t>
   </si>
   <si>
-    <t>BESTEST Cooling 061027d (work around for NaN on COP calc)</t>
+    <t>BESTEST Cooling 061027g  (fixing var names)</t>
   </si>
 </sst>
 </file>
@@ -8713,8 +8713,8 @@
   <dimension ref="A1:M152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A96" sqref="A96:XFD119"/>
+      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
filtering of feb results for 5-3a now done post processing vs. in run
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -2647,7 +2647,7 @@
     <t>bestest_ce_reporting.apr_dec_rh_min_hr</t>
   </si>
   <si>
-    <t>BESTEST Cooling 061027g  (fixing var names)</t>
+    <t>BESTEST Cooling 061028a  (post processing feb results)</t>
   </si>
 </sst>
 </file>
@@ -6441,7 +6441,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
fixed units for 0628 and converted strings to numbers
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -2647,7 +2647,7 @@
     <t>bestest_ce_reporting.apr_dec_rh_min_hr</t>
   </si>
   <si>
-    <t>BESTEST Cooling 061028a  (post processing feb results)</t>
+    <t>BESTEST Cooling 061028c  (fixing units on 0628 hourly)</t>
   </si>
 </sst>
 </file>
@@ -6441,7 +6441,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
fixes to fan and coil inputs re issue #34
This included curves. Effected CE1xx and CE2xx cases
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="23460" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="51200" windowHeight="28260" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2647,7 +2647,7 @@
     <t>bestest_ce_reporting.apr_dec_rh_min_hr</t>
   </si>
   <si>
-    <t>BESTEST Cooling 061028c  (fixing units on 0628 hourly)</t>
+    <t>BESTEST Cooling 061028h  (adding logic for fan schedule based on case num)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
fixing curves for CE cases
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="51200" windowHeight="28260" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2647,7 +2647,7 @@
     <t>bestest_ce_reporting.apr_dec_rh_min_hr</t>
   </si>
   <si>
-    <t>BESTEST Cooling 061028j  (updating reporting for total max and fan cycling for 3x and 4x)</t>
+    <t>BESTEST Cooling 061031b (reversing curves between CE1xx and CE3xx)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
fix error introduced in last commit
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -2647,7 +2647,7 @@
     <t>bestest_ce_reporting.apr_dec_rh_min_hr</t>
   </si>
   <si>
-    <t>BESTEST Cooling 061031d faun_cycylcing)</t>
+    <t>BESTEST Cooling 061031f (fan_cycylcing fixing CE 1x and 2x that I broke)</t>
   </si>
 </sst>
 </file>
@@ -6441,7 +6441,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Fixing fan reporting and EDB EWB
related to issues #16 and #36
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -2647,7 +2647,7 @@
     <t>bestest_ce_reporting.apr_dec_rh_min_hr</t>
   </si>
   <si>
-    <t>BESTEST Cooling 061031f (fan_cycylcing fixing CE 1x and 2x that I broke)</t>
+    <t>BESTEST Cooling 061031k (more fan reporting)</t>
   </si>
 </sst>
 </file>
@@ -6441,7 +6441,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
COP2 fixes issue #42
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="23460" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2647,7 +2647,7 @@
     <t>bestest_ce_reporting.apr_dec_rh_min_hr</t>
   </si>
   <si>
-    <t>BESTEST Cooling 061031n (mean cop2)</t>
+    <t>BESTEST Cooling 061031q (misc cop2 fixes)</t>
   </si>
 </sst>
 </file>
@@ -6441,7 +6441,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
fixing EDB and EWB issue #36
</commit_message>
<xml_diff>
--- a/integration_testing/projects/bestest_CE01.xlsx
+++ b/integration_testing/projects/bestest_CE01.xlsx
@@ -2647,7 +2647,7 @@
     <t>bestest_ce_reporting.apr_dec_rh_min_hr</t>
   </si>
   <si>
-    <t>BESTEST Cooling 061031q (misc cop2 fixes)</t>
+    <t>BESTEST Cooling 061101b (EDB EWB)</t>
   </si>
 </sst>
 </file>
@@ -6441,7 +6441,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>